<commit_message>
lexical analyzer modified, syntax analyzer done with partial test
</commit_message>
<xml_diff>
--- a/regular expression/DFATable.xlsx
+++ b/regular expression/DFATable.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genius-park/Desktop/compilerPrj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genius-park/Desktop/compilerPrj/regular expression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E836A6-FC95-F745-A914-D67DF92022C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE46B52-FEB8-6E44-BF28-75D30C049764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6317B4AA-360D-7446-A49F-9BC5DAD8FE09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
   <si>
     <t>-</t>
   </si>
@@ -77,27 +77,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>WHITESPACE</t>
-  </si>
-  <si>
-    <t>ASSIGN</t>
-  </si>
-  <si>
-    <t>COMP</t>
-  </si>
-  <si>
-    <t>VTYPE</t>
-  </si>
-  <si>
-    <t>NUM</t>
-  </si>
-  <si>
-    <t>STRING</t>
-  </si>
-  <si>
-    <t>CHAR</t>
-  </si>
-  <si>
     <t>;</t>
   </si>
   <si>
@@ -116,27 +95,6 @@
     <t>}</t>
   </si>
   <si>
-    <t>SEMI</t>
-  </si>
-  <si>
-    <t>COMMA</t>
-  </si>
-  <si>
-    <t>LPAREN</t>
-  </si>
-  <si>
-    <t>RPAREN</t>
-  </si>
-  <si>
-    <t>LBRACE</t>
-  </si>
-  <si>
-    <t>RBRACE</t>
-  </si>
-  <si>
-    <t>ARITHMERIC</t>
-  </si>
-  <si>
     <t>\t</t>
   </si>
   <si>
@@ -288,6 +246,57 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>endmark</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>whitespace</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>comp</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>semi</t>
+  </si>
+  <si>
+    <t>comma</t>
+  </si>
+  <si>
+    <t>lparen</t>
+  </si>
+  <si>
+    <t>rparen</t>
+  </si>
+  <si>
+    <t>lbrace</t>
+  </si>
+  <si>
+    <t>rbrace</t>
+  </si>
+  <si>
+    <t>addsub</t>
+  </si>
+  <si>
+    <t>multidiv</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -343,7 +352,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -366,11 +375,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,7 +407,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,10 +731,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F48278F-A549-804C-999D-E15CBB151350}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:CE41"/>
+  <dimension ref="A1:CF42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,7 +742,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
@@ -742,160 +770,160 @@
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="AE1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="AV1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AY1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AZ1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="BA1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="BB1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="BC1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="BD1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="BE1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="BF1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="BG1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="BH1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="BI1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BJ1" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="BK1" s="3">
         <v>0</v>
@@ -931,10 +959,10 @@
         <v>4</v>
       </c>
       <c r="BV1" s="5" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="BW1" s="5" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="BX1" s="3" t="s">
         <v>9</v>
@@ -943,25 +971,28 @@
         <v>10</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="CA1" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="CB1" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="CC1" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="CD1" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="CE1" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="CF1" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1209,13 +1240,16 @@
       <c r="CE2" s="1">
         <v>39</v>
       </c>
+      <c r="CF2" s="1">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1298,13 +1332,14 @@
       <c r="CC3" s="1"/>
       <c r="CD3" s="1"/>
       <c r="CE3" s="1"/>
+      <c r="CF3" s="1"/>
     </row>
-    <row r="4" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1405,13 +1440,14 @@
       <c r="CC4" s="1"/>
       <c r="CD4" s="1"/>
       <c r="CE4" s="1"/>
+      <c r="CF4" s="1"/>
     </row>
-    <row r="5" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
@@ -1514,13 +1550,14 @@
       <c r="CC5" s="1"/>
       <c r="CD5" s="1"/>
       <c r="CE5" s="1"/>
+      <c r="CF5" s="1"/>
     </row>
-    <row r="6" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1623,13 +1660,14 @@
       <c r="CC6" s="1"/>
       <c r="CD6" s="1"/>
       <c r="CE6" s="1"/>
+      <c r="CF6" s="1"/>
     </row>
-    <row r="7" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1712,13 +1750,14 @@
       <c r="CC7" s="1"/>
       <c r="CD7" s="1"/>
       <c r="CE7" s="1"/>
+      <c r="CF7" s="1"/>
     </row>
-    <row r="8" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1801,13 +1840,14 @@
       <c r="CC8" s="1"/>
       <c r="CD8" s="1"/>
       <c r="CE8" s="1"/>
+      <c r="CF8" s="1"/>
     </row>
-    <row r="9" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1890,13 +1930,14 @@
       <c r="CC9" s="1"/>
       <c r="CD9" s="1"/>
       <c r="CE9" s="1"/>
+      <c r="CF9" s="1"/>
     </row>
-    <row r="10" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1979,13 +2020,14 @@
       <c r="CC10" s="1"/>
       <c r="CD10" s="1"/>
       <c r="CE10" s="1"/>
+      <c r="CF10" s="1"/>
     </row>
-    <row r="11" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2068,13 +2110,14 @@
       <c r="CC11" s="1"/>
       <c r="CD11" s="1"/>
       <c r="CE11" s="1"/>
+      <c r="CF11" s="1"/>
     </row>
-    <row r="12" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2159,13 +2202,14 @@
       <c r="CC12" s="1"/>
       <c r="CD12" s="1"/>
       <c r="CE12" s="1"/>
+      <c r="CF12" s="1"/>
     </row>
-    <row r="13" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2248,12 +2292,15 @@
       <c r="CC13" s="1"/>
       <c r="CD13" s="1"/>
       <c r="CE13" s="1"/>
+      <c r="CF13" s="1"/>
     </row>
-    <row r="14" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2337,13 +2384,14 @@
       <c r="CC14" s="1"/>
       <c r="CD14" s="1"/>
       <c r="CE14" s="1"/>
+      <c r="CF14" s="1"/>
     </row>
-    <row r="15" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2426,13 +2474,14 @@
       <c r="CC15" s="1"/>
       <c r="CD15" s="1"/>
       <c r="CE15" s="1"/>
+      <c r="CF15" s="1"/>
     </row>
-    <row r="16" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2517,13 +2566,14 @@
       <c r="CC16" s="1"/>
       <c r="CD16" s="1"/>
       <c r="CE16" s="1"/>
+      <c r="CF16" s="1"/>
     </row>
-    <row r="17" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2606,13 +2656,14 @@
       <c r="CC17" s="1"/>
       <c r="CD17" s="1"/>
       <c r="CE17" s="1"/>
+      <c r="CF17" s="1"/>
     </row>
-    <row r="18" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2697,13 +2748,14 @@
       <c r="CC18" s="1"/>
       <c r="CD18" s="1"/>
       <c r="CE18" s="1"/>
+      <c r="CF18" s="1"/>
     </row>
-    <row r="19" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2786,13 +2838,14 @@
       <c r="CC19" s="1"/>
       <c r="CD19" s="1"/>
       <c r="CE19" s="1"/>
+      <c r="CF19" s="1"/>
     </row>
-    <row r="20" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2999,13 +3052,14 @@
       <c r="CC20" s="1"/>
       <c r="CD20" s="1"/>
       <c r="CE20" s="1"/>
+      <c r="CF20" s="1"/>
     </row>
-    <row r="21" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -3212,13 +3266,14 @@
       <c r="CC21" s="1"/>
       <c r="CD21" s="1"/>
       <c r="CE21" s="1"/>
+      <c r="CF21" s="1"/>
     </row>
-    <row r="22" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -3425,12 +3480,15 @@
       <c r="CC22" s="1"/>
       <c r="CD22" s="1"/>
       <c r="CE22" s="1"/>
+      <c r="CF22" s="1"/>
     </row>
-    <row r="23" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -3640,12 +3698,15 @@
       <c r="CC23" s="1"/>
       <c r="CD23" s="1"/>
       <c r="CE23" s="1"/>
+      <c r="CF23" s="1"/>
     </row>
-    <row r="24" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -3855,12 +3916,15 @@
       <c r="CC24" s="1"/>
       <c r="CD24" s="1"/>
       <c r="CE24" s="1"/>
+      <c r="CF24" s="1"/>
     </row>
-    <row r="25" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -4070,12 +4134,15 @@
       <c r="CC25" s="1"/>
       <c r="CD25" s="1"/>
       <c r="CE25" s="1"/>
+      <c r="CF25" s="1"/>
     </row>
-    <row r="26" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -4285,13 +4352,14 @@
       <c r="CC26" s="1"/>
       <c r="CD26" s="1"/>
       <c r="CE26" s="1"/>
+      <c r="CF26" s="1"/>
     </row>
-    <row r="27" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -4374,12 +4442,15 @@
       <c r="CC27" s="1"/>
       <c r="CD27" s="1"/>
       <c r="CE27" s="1"/>
+      <c r="CF27" s="1"/>
     </row>
-    <row r="28" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -4587,12 +4658,15 @@
       <c r="CC28" s="1"/>
       <c r="CD28" s="1"/>
       <c r="CE28" s="1"/>
+      <c r="CF28" s="1"/>
     </row>
-    <row r="29" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -4676,12 +4750,15 @@
       <c r="CC29" s="1"/>
       <c r="CD29" s="1"/>
       <c r="CE29" s="1"/>
+      <c r="CF29" s="1"/>
     </row>
-    <row r="30" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -4765,12 +4842,15 @@
       <c r="CC30" s="1"/>
       <c r="CD30" s="1"/>
       <c r="CE30" s="1"/>
+      <c r="CF30" s="1"/>
     </row>
-    <row r="31" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -4854,13 +4934,14 @@
       <c r="CC31" s="1"/>
       <c r="CD31" s="1"/>
       <c r="CE31" s="1"/>
+      <c r="CF31" s="1"/>
     </row>
-    <row r="32" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -4943,13 +5024,14 @@
       <c r="CC32" s="1"/>
       <c r="CD32" s="1"/>
       <c r="CE32" s="1"/>
+      <c r="CF32" s="1"/>
     </row>
-    <row r="33" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -5032,13 +5114,14 @@
       <c r="CC33" s="1"/>
       <c r="CD33" s="1"/>
       <c r="CE33" s="1"/>
+      <c r="CF33" s="1"/>
     </row>
-    <row r="34" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -5141,13 +5224,14 @@
       <c r="CC34" s="1"/>
       <c r="CD34" s="1"/>
       <c r="CE34" s="1"/>
+      <c r="CF34" s="1"/>
     </row>
-    <row r="35" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -5250,540 +5334,637 @@
       <c r="CC35" s="1"/>
       <c r="CD35" s="1"/>
       <c r="CE35" s="1"/>
+      <c r="CF35" s="1"/>
     </row>
-    <row r="36" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
-      <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-      <c r="AA36" s="6"/>
-      <c r="AB36" s="6"/>
-      <c r="AC36" s="6"/>
-      <c r="AD36" s="6"/>
-      <c r="AE36" s="6"/>
-      <c r="AF36" s="6"/>
-      <c r="AG36" s="6"/>
-      <c r="AH36" s="6"/>
-      <c r="AI36" s="6"/>
-      <c r="AJ36" s="6"/>
-      <c r="AK36" s="6"/>
-      <c r="AL36" s="6"/>
-      <c r="AM36" s="6"/>
-      <c r="AN36" s="6"/>
-      <c r="AO36" s="6"/>
-      <c r="AP36" s="6"/>
-      <c r="AQ36" s="6"/>
-      <c r="AR36" s="6"/>
-      <c r="AS36" s="6"/>
-      <c r="AT36" s="6"/>
-      <c r="AU36" s="6"/>
-      <c r="AV36" s="6"/>
-      <c r="AW36" s="6"/>
-      <c r="AX36" s="6"/>
-      <c r="AY36" s="6"/>
-      <c r="AZ36" s="6"/>
-      <c r="BA36" s="6"/>
-      <c r="BB36" s="6"/>
-      <c r="BC36" s="6"/>
-      <c r="BD36" s="6"/>
-      <c r="BE36" s="6"/>
-      <c r="BF36" s="6"/>
-      <c r="BG36" s="6"/>
-      <c r="BH36" s="6"/>
-      <c r="BI36" s="6"/>
-      <c r="BJ36" s="6"/>
-      <c r="BK36" s="6"/>
-      <c r="BL36" s="6"/>
-      <c r="BM36" s="6"/>
-      <c r="BN36" s="6"/>
-      <c r="BO36" s="6"/>
-      <c r="BP36" s="6"/>
-      <c r="BQ36" s="6"/>
-      <c r="BR36" s="6"/>
-      <c r="BS36" s="6"/>
-      <c r="BT36" s="6"/>
-      <c r="BU36" s="6"/>
-      <c r="BV36" s="6"/>
-      <c r="BW36" s="6"/>
-      <c r="BX36" s="6"/>
-      <c r="BY36" s="6"/>
-      <c r="BZ36" s="6"/>
-      <c r="CA36" s="6"/>
-      <c r="CB36" s="6"/>
-      <c r="CC36" s="6"/>
-      <c r="CD36" s="6"/>
-      <c r="CE36" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="1"/>
+      <c r="AG36" s="1"/>
+      <c r="AH36" s="1"/>
+      <c r="AI36" s="1"/>
+      <c r="AJ36" s="1"/>
+      <c r="AK36" s="1"/>
+      <c r="AL36" s="1"/>
+      <c r="AM36" s="1"/>
+      <c r="AN36" s="1"/>
+      <c r="AO36" s="1"/>
+      <c r="AP36" s="1"/>
+      <c r="AQ36" s="1"/>
+      <c r="AR36" s="1"/>
+      <c r="AS36" s="1"/>
+      <c r="AT36" s="1"/>
+      <c r="AU36" s="1"/>
+      <c r="AV36" s="1"/>
+      <c r="AW36" s="1"/>
+      <c r="AX36" s="1"/>
+      <c r="AY36" s="1"/>
+      <c r="AZ36" s="1"/>
+      <c r="BA36" s="1"/>
+      <c r="BB36" s="1"/>
+      <c r="BC36" s="1"/>
+      <c r="BD36" s="1"/>
+      <c r="BE36" s="1"/>
+      <c r="BF36" s="1"/>
+      <c r="BG36" s="1"/>
+      <c r="BH36" s="1"/>
+      <c r="BI36" s="1"/>
+      <c r="BJ36" s="1"/>
+      <c r="BK36" s="1"/>
+      <c r="BL36" s="1"/>
+      <c r="BM36" s="1"/>
+      <c r="BN36" s="1"/>
+      <c r="BO36" s="1"/>
+      <c r="BP36" s="1"/>
+      <c r="BQ36" s="1"/>
+      <c r="BR36" s="1"/>
+      <c r="BS36" s="1"/>
+      <c r="BT36" s="1"/>
+      <c r="BU36" s="1"/>
+      <c r="BV36" s="1"/>
+      <c r="BW36" s="1"/>
+      <c r="BX36" s="1"/>
+      <c r="BY36" s="1"/>
+      <c r="BZ36" s="1"/>
+      <c r="CA36" s="1"/>
+      <c r="CB36" s="1"/>
+      <c r="CC36" s="1"/>
+      <c r="CD36" s="1"/>
+      <c r="CE36" s="1"/>
+      <c r="CF36" s="1"/>
     </row>
-    <row r="37" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
-      <c r="U37" s="6"/>
-      <c r="V37" s="6"/>
-      <c r="W37" s="6"/>
-      <c r="X37" s="6"/>
-      <c r="Y37" s="6"/>
-      <c r="Z37" s="6"/>
-      <c r="AA37" s="6"/>
-      <c r="AB37" s="6"/>
-      <c r="AC37" s="6"/>
-      <c r="AD37" s="6"/>
-      <c r="AE37" s="6"/>
-      <c r="AF37" s="6"/>
-      <c r="AG37" s="6"/>
-      <c r="AH37" s="6"/>
-      <c r="AI37" s="6"/>
-      <c r="AJ37" s="6"/>
-      <c r="AK37" s="6"/>
-      <c r="AL37" s="6"/>
-      <c r="AM37" s="6"/>
-      <c r="AN37" s="6"/>
-      <c r="AO37" s="6"/>
-      <c r="AP37" s="6"/>
-      <c r="AQ37" s="6"/>
-      <c r="AR37" s="6"/>
-      <c r="AS37" s="6"/>
-      <c r="AT37" s="6"/>
-      <c r="AU37" s="6"/>
-      <c r="AV37" s="6"/>
-      <c r="AW37" s="6"/>
-      <c r="AX37" s="6"/>
-      <c r="AY37" s="6"/>
-      <c r="AZ37" s="6"/>
-      <c r="BA37" s="6"/>
-      <c r="BB37" s="6"/>
-      <c r="BC37" s="6"/>
-      <c r="BD37" s="6"/>
-      <c r="BE37" s="6"/>
-      <c r="BF37" s="6"/>
-      <c r="BG37" s="6"/>
-      <c r="BH37" s="6"/>
-      <c r="BI37" s="6"/>
-      <c r="BJ37" s="6"/>
-      <c r="BK37" s="6"/>
-      <c r="BL37" s="6"/>
-      <c r="BM37" s="6"/>
-      <c r="BN37" s="6"/>
-      <c r="BO37" s="6"/>
-      <c r="BP37" s="6"/>
-      <c r="BQ37" s="6"/>
-      <c r="BR37" s="6"/>
-      <c r="BS37" s="6"/>
-      <c r="BT37" s="6"/>
-      <c r="BU37" s="6"/>
-      <c r="BV37" s="6"/>
-      <c r="BW37" s="6"/>
-      <c r="BX37" s="6"/>
-      <c r="BY37" s="6"/>
-      <c r="BZ37" s="6"/>
-      <c r="CA37" s="6"/>
-      <c r="CB37" s="6"/>
-      <c r="CC37" s="6"/>
-      <c r="CD37" s="6"/>
-      <c r="CE37" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
+      <c r="AH37" s="1"/>
+      <c r="AI37" s="1"/>
+      <c r="AJ37" s="1"/>
+      <c r="AK37" s="1"/>
+      <c r="AL37" s="1"/>
+      <c r="AM37" s="1"/>
+      <c r="AN37" s="1"/>
+      <c r="AO37" s="1"/>
+      <c r="AP37" s="1"/>
+      <c r="AQ37" s="1"/>
+      <c r="AR37" s="1"/>
+      <c r="AS37" s="1"/>
+      <c r="AT37" s="1"/>
+      <c r="AU37" s="1"/>
+      <c r="AV37" s="1"/>
+      <c r="AW37" s="1"/>
+      <c r="AX37" s="1"/>
+      <c r="AY37" s="1"/>
+      <c r="AZ37" s="1"/>
+      <c r="BA37" s="1"/>
+      <c r="BB37" s="1"/>
+      <c r="BC37" s="1"/>
+      <c r="BD37" s="1"/>
+      <c r="BE37" s="1"/>
+      <c r="BF37" s="1"/>
+      <c r="BG37" s="1"/>
+      <c r="BH37" s="1"/>
+      <c r="BI37" s="1"/>
+      <c r="BJ37" s="1"/>
+      <c r="BK37" s="1"/>
+      <c r="BL37" s="1"/>
+      <c r="BM37" s="1"/>
+      <c r="BN37" s="1"/>
+      <c r="BO37" s="1"/>
+      <c r="BP37" s="1"/>
+      <c r="BQ37" s="1"/>
+      <c r="BR37" s="1"/>
+      <c r="BS37" s="1"/>
+      <c r="BT37" s="1"/>
+      <c r="BU37" s="1"/>
+      <c r="BV37" s="1"/>
+      <c r="BW37" s="1"/>
+      <c r="BX37" s="1"/>
+      <c r="BY37" s="1"/>
+      <c r="BZ37" s="1"/>
+      <c r="CA37" s="1"/>
+      <c r="CB37" s="1"/>
+      <c r="CC37" s="1"/>
+      <c r="CD37" s="1"/>
+      <c r="CE37" s="1"/>
+      <c r="CF37" s="1"/>
     </row>
-    <row r="38" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
-      <c r="U38" s="6"/>
-      <c r="V38" s="6"/>
-      <c r="W38" s="6"/>
-      <c r="X38" s="6"/>
-      <c r="Y38" s="6"/>
-      <c r="Z38" s="6"/>
-      <c r="AA38" s="6"/>
-      <c r="AB38" s="6"/>
-      <c r="AC38" s="6"/>
-      <c r="AD38" s="6"/>
-      <c r="AE38" s="6"/>
-      <c r="AF38" s="6"/>
-      <c r="AG38" s="6"/>
-      <c r="AH38" s="6"/>
-      <c r="AI38" s="6"/>
-      <c r="AJ38" s="6"/>
-      <c r="AK38" s="6"/>
-      <c r="AL38" s="6"/>
-      <c r="AM38" s="6"/>
-      <c r="AN38" s="6"/>
-      <c r="AO38" s="6"/>
-      <c r="AP38" s="6"/>
-      <c r="AQ38" s="6"/>
-      <c r="AR38" s="6"/>
-      <c r="AS38" s="6"/>
-      <c r="AT38" s="6"/>
-      <c r="AU38" s="6"/>
-      <c r="AV38" s="6"/>
-      <c r="AW38" s="6"/>
-      <c r="AX38" s="6"/>
-      <c r="AY38" s="6"/>
-      <c r="AZ38" s="6"/>
-      <c r="BA38" s="6"/>
-      <c r="BB38" s="6"/>
-      <c r="BC38" s="6"/>
-      <c r="BD38" s="6"/>
-      <c r="BE38" s="6"/>
-      <c r="BF38" s="6"/>
-      <c r="BG38" s="6"/>
-      <c r="BH38" s="6"/>
-      <c r="BI38" s="6"/>
-      <c r="BJ38" s="6"/>
-      <c r="BK38" s="6"/>
-      <c r="BL38" s="6"/>
-      <c r="BM38" s="6"/>
-      <c r="BN38" s="6"/>
-      <c r="BO38" s="6"/>
-      <c r="BP38" s="6"/>
-      <c r="BQ38" s="6"/>
-      <c r="BR38" s="6"/>
-      <c r="BS38" s="6"/>
-      <c r="BT38" s="6"/>
-      <c r="BU38" s="6"/>
-      <c r="BV38" s="6"/>
-      <c r="BW38" s="6"/>
-      <c r="BX38" s="6"/>
-      <c r="BY38" s="6"/>
-      <c r="BZ38" s="6"/>
-      <c r="CA38" s="6"/>
-      <c r="CB38" s="6"/>
-      <c r="CC38" s="6"/>
-      <c r="CD38" s="6"/>
-      <c r="CE38" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
+      <c r="AH38" s="1"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
+      <c r="AK38" s="1"/>
+      <c r="AL38" s="1"/>
+      <c r="AM38" s="1"/>
+      <c r="AN38" s="1"/>
+      <c r="AO38" s="1"/>
+      <c r="AP38" s="1"/>
+      <c r="AQ38" s="1"/>
+      <c r="AR38" s="1"/>
+      <c r="AS38" s="1"/>
+      <c r="AT38" s="1"/>
+      <c r="AU38" s="1"/>
+      <c r="AV38" s="1"/>
+      <c r="AW38" s="1"/>
+      <c r="AX38" s="1"/>
+      <c r="AY38" s="1"/>
+      <c r="AZ38" s="1"/>
+      <c r="BA38" s="1"/>
+      <c r="BB38" s="1"/>
+      <c r="BC38" s="1"/>
+      <c r="BD38" s="1"/>
+      <c r="BE38" s="1"/>
+      <c r="BF38" s="1"/>
+      <c r="BG38" s="1"/>
+      <c r="BH38" s="1"/>
+      <c r="BI38" s="1"/>
+      <c r="BJ38" s="1"/>
+      <c r="BK38" s="1"/>
+      <c r="BL38" s="1"/>
+      <c r="BM38" s="1"/>
+      <c r="BN38" s="1"/>
+      <c r="BO38" s="1"/>
+      <c r="BP38" s="1"/>
+      <c r="BQ38" s="1"/>
+      <c r="BR38" s="1"/>
+      <c r="BS38" s="1"/>
+      <c r="BT38" s="1"/>
+      <c r="BU38" s="1"/>
+      <c r="BV38" s="1"/>
+      <c r="BW38" s="1"/>
+      <c r="BX38" s="1"/>
+      <c r="BY38" s="1"/>
+      <c r="BZ38" s="1"/>
+      <c r="CA38" s="1"/>
+      <c r="CB38" s="1"/>
+      <c r="CC38" s="1"/>
+      <c r="CD38" s="1"/>
+      <c r="CE38" s="1"/>
+      <c r="CF38" s="1"/>
     </row>
-    <row r="39" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="6"/>
-      <c r="U39" s="6"/>
-      <c r="V39" s="6"/>
-      <c r="W39" s="6"/>
-      <c r="X39" s="6"/>
-      <c r="Y39" s="6"/>
-      <c r="Z39" s="6"/>
-      <c r="AA39" s="6"/>
-      <c r="AB39" s="6"/>
-      <c r="AC39" s="6"/>
-      <c r="AD39" s="6"/>
-      <c r="AE39" s="6"/>
-      <c r="AF39" s="6"/>
-      <c r="AG39" s="6"/>
-      <c r="AH39" s="6"/>
-      <c r="AI39" s="6"/>
-      <c r="AJ39" s="6"/>
-      <c r="AK39" s="6"/>
-      <c r="AL39" s="6"/>
-      <c r="AM39" s="6"/>
-      <c r="AN39" s="6"/>
-      <c r="AO39" s="6"/>
-      <c r="AP39" s="6"/>
-      <c r="AQ39" s="6"/>
-      <c r="AR39" s="6"/>
-      <c r="AS39" s="6"/>
-      <c r="AT39" s="6"/>
-      <c r="AU39" s="6"/>
-      <c r="AV39" s="6"/>
-      <c r="AW39" s="6"/>
-      <c r="AX39" s="6"/>
-      <c r="AY39" s="6"/>
-      <c r="AZ39" s="6"/>
-      <c r="BA39" s="6"/>
-      <c r="BB39" s="6"/>
-      <c r="BC39" s="6"/>
-      <c r="BD39" s="6"/>
-      <c r="BE39" s="6"/>
-      <c r="BF39" s="6"/>
-      <c r="BG39" s="6"/>
-      <c r="BH39" s="6"/>
-      <c r="BI39" s="6"/>
-      <c r="BJ39" s="6"/>
-      <c r="BK39" s="6"/>
-      <c r="BL39" s="6"/>
-      <c r="BM39" s="6"/>
-      <c r="BN39" s="6"/>
-      <c r="BO39" s="6"/>
-      <c r="BP39" s="6"/>
-      <c r="BQ39" s="6"/>
-      <c r="BR39" s="6"/>
-      <c r="BS39" s="6"/>
-      <c r="BT39" s="6"/>
-      <c r="BU39" s="6"/>
-      <c r="BV39" s="6"/>
-      <c r="BW39" s="6"/>
-      <c r="BX39" s="6"/>
-      <c r="BY39" s="6"/>
-      <c r="BZ39" s="6"/>
-      <c r="CA39" s="6"/>
-      <c r="CB39" s="6"/>
-      <c r="CC39" s="6"/>
-      <c r="CD39" s="6"/>
-      <c r="CE39" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="1"/>
+      <c r="AH39" s="1"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
+      <c r="AK39" s="1"/>
+      <c r="AL39" s="1"/>
+      <c r="AM39" s="1"/>
+      <c r="AN39" s="1"/>
+      <c r="AO39" s="1"/>
+      <c r="AP39" s="1"/>
+      <c r="AQ39" s="1"/>
+      <c r="AR39" s="1"/>
+      <c r="AS39" s="1"/>
+      <c r="AT39" s="1"/>
+      <c r="AU39" s="1"/>
+      <c r="AV39" s="1"/>
+      <c r="AW39" s="1"/>
+      <c r="AX39" s="1"/>
+      <c r="AY39" s="1"/>
+      <c r="AZ39" s="1"/>
+      <c r="BA39" s="1"/>
+      <c r="BB39" s="1"/>
+      <c r="BC39" s="1"/>
+      <c r="BD39" s="1"/>
+      <c r="BE39" s="1"/>
+      <c r="BF39" s="1"/>
+      <c r="BG39" s="1"/>
+      <c r="BH39" s="1"/>
+      <c r="BI39" s="1"/>
+      <c r="BJ39" s="1"/>
+      <c r="BK39" s="1"/>
+      <c r="BL39" s="1"/>
+      <c r="BM39" s="1"/>
+      <c r="BN39" s="1"/>
+      <c r="BO39" s="1"/>
+      <c r="BP39" s="1"/>
+      <c r="BQ39" s="1"/>
+      <c r="BR39" s="1"/>
+      <c r="BS39" s="1"/>
+      <c r="BT39" s="1"/>
+      <c r="BU39" s="1"/>
+      <c r="BV39" s="1"/>
+      <c r="BW39" s="1"/>
+      <c r="BX39" s="1"/>
+      <c r="BY39" s="1"/>
+      <c r="BZ39" s="1"/>
+      <c r="CA39" s="1"/>
+      <c r="CB39" s="1"/>
+      <c r="CC39" s="1"/>
+      <c r="CD39" s="1"/>
+      <c r="CE39" s="1"/>
+      <c r="CF39" s="1"/>
     </row>
-    <row r="40" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="6"/>
-      <c r="U40" s="6"/>
-      <c r="V40" s="6"/>
-      <c r="W40" s="6"/>
-      <c r="X40" s="6"/>
-      <c r="Y40" s="6"/>
-      <c r="Z40" s="6"/>
-      <c r="AA40" s="6"/>
-      <c r="AB40" s="6"/>
-      <c r="AC40" s="6"/>
-      <c r="AD40" s="6"/>
-      <c r="AE40" s="6"/>
-      <c r="AF40" s="6"/>
-      <c r="AG40" s="6"/>
-      <c r="AH40" s="6"/>
-      <c r="AI40" s="6"/>
-      <c r="AJ40" s="6"/>
-      <c r="AK40" s="6"/>
-      <c r="AL40" s="6"/>
-      <c r="AM40" s="6"/>
-      <c r="AN40" s="6"/>
-      <c r="AO40" s="6"/>
-      <c r="AP40" s="6"/>
-      <c r="AQ40" s="6"/>
-      <c r="AR40" s="6"/>
-      <c r="AS40" s="6"/>
-      <c r="AT40" s="6"/>
-      <c r="AU40" s="6"/>
-      <c r="AV40" s="6"/>
-      <c r="AW40" s="6"/>
-      <c r="AX40" s="6"/>
-      <c r="AY40" s="6"/>
-      <c r="AZ40" s="6"/>
-      <c r="BA40" s="6"/>
-      <c r="BB40" s="6"/>
-      <c r="BC40" s="6"/>
-      <c r="BD40" s="6"/>
-      <c r="BE40" s="6"/>
-      <c r="BF40" s="6"/>
-      <c r="BG40" s="6"/>
-      <c r="BH40" s="6"/>
-      <c r="BI40" s="6"/>
-      <c r="BJ40" s="6"/>
-      <c r="BK40" s="6"/>
-      <c r="BL40" s="6"/>
-      <c r="BM40" s="6"/>
-      <c r="BN40" s="6"/>
-      <c r="BO40" s="6"/>
-      <c r="BP40" s="6"/>
-      <c r="BQ40" s="6"/>
-      <c r="BR40" s="6"/>
-      <c r="BS40" s="6"/>
-      <c r="BT40" s="6"/>
-      <c r="BU40" s="6"/>
-      <c r="BV40" s="6"/>
-      <c r="BW40" s="6"/>
-      <c r="BX40" s="6"/>
-      <c r="BY40" s="6"/>
-      <c r="BZ40" s="6"/>
-      <c r="CA40" s="6"/>
-      <c r="CB40" s="6"/>
-      <c r="CC40" s="6"/>
-      <c r="CD40" s="6"/>
-      <c r="CE40" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1"/>
+      <c r="AD40" s="1"/>
+      <c r="AE40" s="1"/>
+      <c r="AF40" s="1"/>
+      <c r="AG40" s="1"/>
+      <c r="AH40" s="1"/>
+      <c r="AI40" s="1"/>
+      <c r="AJ40" s="1"/>
+      <c r="AK40" s="1"/>
+      <c r="AL40" s="1"/>
+      <c r="AM40" s="1"/>
+      <c r="AN40" s="1"/>
+      <c r="AO40" s="1"/>
+      <c r="AP40" s="1"/>
+      <c r="AQ40" s="1"/>
+      <c r="AR40" s="1"/>
+      <c r="AS40" s="1"/>
+      <c r="AT40" s="1"/>
+      <c r="AU40" s="1"/>
+      <c r="AV40" s="1"/>
+      <c r="AW40" s="1"/>
+      <c r="AX40" s="1"/>
+      <c r="AY40" s="1"/>
+      <c r="AZ40" s="1"/>
+      <c r="BA40" s="1"/>
+      <c r="BB40" s="1"/>
+      <c r="BC40" s="1"/>
+      <c r="BD40" s="1"/>
+      <c r="BE40" s="1"/>
+      <c r="BF40" s="1"/>
+      <c r="BG40" s="1"/>
+      <c r="BH40" s="1"/>
+      <c r="BI40" s="1"/>
+      <c r="BJ40" s="1"/>
+      <c r="BK40" s="1"/>
+      <c r="BL40" s="1"/>
+      <c r="BM40" s="1"/>
+      <c r="BN40" s="1"/>
+      <c r="BO40" s="1"/>
+      <c r="BP40" s="1"/>
+      <c r="BQ40" s="1"/>
+      <c r="BR40" s="1"/>
+      <c r="BS40" s="1"/>
+      <c r="BT40" s="1"/>
+      <c r="BU40" s="1"/>
+      <c r="BV40" s="1"/>
+      <c r="BW40" s="1"/>
+      <c r="BX40" s="1"/>
+      <c r="BY40" s="1"/>
+      <c r="BZ40" s="1"/>
+      <c r="CA40" s="1"/>
+      <c r="CB40" s="1"/>
+      <c r="CC40" s="1"/>
+      <c r="CD40" s="1"/>
+      <c r="CE40" s="1"/>
+      <c r="CF40" s="1"/>
     </row>
-    <row r="41" spans="1:83" ht="20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:84" ht="20" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="6"/>
-      <c r="T41" s="6"/>
-      <c r="U41" s="6"/>
-      <c r="V41" s="6"/>
-      <c r="W41" s="6"/>
-      <c r="X41" s="6"/>
-      <c r="Y41" s="6"/>
-      <c r="Z41" s="6"/>
-      <c r="AA41" s="6"/>
-      <c r="AB41" s="6"/>
-      <c r="AC41" s="6"/>
-      <c r="AD41" s="6"/>
-      <c r="AE41" s="6"/>
-      <c r="AF41" s="6"/>
-      <c r="AG41" s="6"/>
-      <c r="AH41" s="6"/>
-      <c r="AI41" s="6"/>
-      <c r="AJ41" s="6"/>
-      <c r="AK41" s="6"/>
-      <c r="AL41" s="6"/>
-      <c r="AM41" s="6"/>
-      <c r="AN41" s="6"/>
-      <c r="AO41" s="6"/>
-      <c r="AP41" s="6"/>
-      <c r="AQ41" s="6"/>
-      <c r="AR41" s="6"/>
-      <c r="AS41" s="6"/>
-      <c r="AT41" s="6"/>
-      <c r="AU41" s="6"/>
-      <c r="AV41" s="6"/>
-      <c r="AW41" s="6"/>
-      <c r="AX41" s="6"/>
-      <c r="AY41" s="6"/>
-      <c r="AZ41" s="6"/>
-      <c r="BA41" s="6"/>
-      <c r="BB41" s="6"/>
-      <c r="BC41" s="6"/>
-      <c r="BD41" s="6"/>
-      <c r="BE41" s="6"/>
-      <c r="BF41" s="6"/>
-      <c r="BG41" s="6"/>
-      <c r="BH41" s="6"/>
-      <c r="BI41" s="6"/>
-      <c r="BJ41" s="6"/>
-      <c r="BK41" s="6"/>
-      <c r="BL41" s="6"/>
-      <c r="BM41" s="6"/>
-      <c r="BN41" s="6"/>
-      <c r="BO41" s="6"/>
-      <c r="BP41" s="6"/>
-      <c r="BQ41" s="6"/>
-      <c r="BR41" s="6"/>
-      <c r="BS41" s="6"/>
-      <c r="BT41" s="6"/>
-      <c r="BU41" s="6"/>
-      <c r="BV41" s="6"/>
-      <c r="BW41" s="6"/>
-      <c r="BX41" s="6"/>
-      <c r="BY41" s="6"/>
-      <c r="BZ41" s="6"/>
-      <c r="CA41" s="6"/>
-      <c r="CB41" s="6"/>
-      <c r="CC41" s="6"/>
-      <c r="CD41" s="6"/>
-      <c r="CE41" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="1"/>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="1"/>
+      <c r="AI41" s="1"/>
+      <c r="AJ41" s="1"/>
+      <c r="AK41" s="1"/>
+      <c r="AL41" s="1"/>
+      <c r="AM41" s="1"/>
+      <c r="AN41" s="1"/>
+      <c r="AO41" s="1"/>
+      <c r="AP41" s="1"/>
+      <c r="AQ41" s="1"/>
+      <c r="AR41" s="1"/>
+      <c r="AS41" s="1"/>
+      <c r="AT41" s="1"/>
+      <c r="AU41" s="1"/>
+      <c r="AV41" s="1"/>
+      <c r="AW41" s="1"/>
+      <c r="AX41" s="1"/>
+      <c r="AY41" s="1"/>
+      <c r="AZ41" s="1"/>
+      <c r="BA41" s="1"/>
+      <c r="BB41" s="1"/>
+      <c r="BC41" s="1"/>
+      <c r="BD41" s="1"/>
+      <c r="BE41" s="1"/>
+      <c r="BF41" s="1"/>
+      <c r="BG41" s="1"/>
+      <c r="BH41" s="1"/>
+      <c r="BI41" s="1"/>
+      <c r="BJ41" s="1"/>
+      <c r="BK41" s="1"/>
+      <c r="BL41" s="1"/>
+      <c r="BM41" s="1"/>
+      <c r="BN41" s="1"/>
+      <c r="BO41" s="1"/>
+      <c r="BP41" s="1"/>
+      <c r="BQ41" s="1"/>
+      <c r="BR41" s="1"/>
+      <c r="BS41" s="1"/>
+      <c r="BT41" s="1"/>
+      <c r="BU41" s="1"/>
+      <c r="BV41" s="1"/>
+      <c r="BW41" s="1"/>
+      <c r="BX41" s="1"/>
+      <c r="BY41" s="1"/>
+      <c r="BZ41" s="1"/>
+      <c r="CA41" s="1"/>
+      <c r="CB41" s="1"/>
+      <c r="CC41" s="1"/>
+      <c r="CD41" s="1"/>
+      <c r="CE41" s="1"/>
+      <c r="CF41" s="1"/>
+    </row>
+    <row r="42" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>40</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
+      <c r="Y42" s="8"/>
+      <c r="Z42" s="8"/>
+      <c r="AA42" s="8"/>
+      <c r="AB42" s="8"/>
+      <c r="AC42" s="8"/>
+      <c r="AD42" s="8"/>
+      <c r="AE42" s="8"/>
+      <c r="AF42" s="8"/>
+      <c r="AG42" s="8"/>
+      <c r="AH42" s="8"/>
+      <c r="AI42" s="8"/>
+      <c r="AJ42" s="8"/>
+      <c r="AK42" s="8"/>
+      <c r="AL42" s="8"/>
+      <c r="AM42" s="8"/>
+      <c r="AN42" s="8"/>
+      <c r="AO42" s="8"/>
+      <c r="AP42" s="8"/>
+      <c r="AQ42" s="8"/>
+      <c r="AR42" s="8"/>
+      <c r="AS42" s="8"/>
+      <c r="AT42" s="8"/>
+      <c r="AU42" s="8"/>
+      <c r="AV42" s="8"/>
+      <c r="AW42" s="8"/>
+      <c r="AX42" s="8"/>
+      <c r="AY42" s="8"/>
+      <c r="AZ42" s="8"/>
+      <c r="BA42" s="8"/>
+      <c r="BB42" s="8"/>
+      <c r="BC42" s="8"/>
+      <c r="BD42" s="8"/>
+      <c r="BE42" s="8"/>
+      <c r="BF42" s="8"/>
+      <c r="BG42" s="8"/>
+      <c r="BH42" s="8"/>
+      <c r="BI42" s="8"/>
+      <c r="BJ42" s="8"/>
+      <c r="BK42" s="8"/>
+      <c r="BL42" s="8"/>
+      <c r="BM42" s="8"/>
+      <c r="BN42" s="8"/>
+      <c r="BO42" s="8"/>
+      <c r="BP42" s="8"/>
+      <c r="BQ42" s="8"/>
+      <c r="BR42" s="8"/>
+      <c r="BS42" s="8"/>
+      <c r="BT42" s="8"/>
+      <c r="BU42" s="8"/>
+      <c r="BV42" s="8"/>
+      <c r="BW42" s="8"/>
+      <c r="BX42" s="8"/>
+      <c r="BY42" s="8"/>
+      <c r="BZ42" s="8"/>
+      <c r="CA42" s="8"/>
+      <c r="CB42" s="8"/>
+      <c r="CC42" s="8"/>
+      <c r="CD42" s="8"/>
+      <c r="CE42" s="8"/>
+      <c r="CF42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
token 'and' and 'or' adde for elaborate condition of while and if
</commit_message>
<xml_diff>
--- a/regular expression/DFATable.xlsx
+++ b/regular expression/DFATable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genius-park/Desktop/compilerPrj/regular expression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE46B52-FEB8-6E44-BF28-75D30C049764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A47FCE9-A47C-7642-9A8B-EBDB8199659C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6317B4AA-360D-7446-A49F-9BC5DAD8FE09}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
   <si>
     <t>-</t>
   </si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>|</t>
   </si>
 </sst>
 </file>
@@ -352,7 +364,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -373,17 +385,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -407,15 +408,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,10 +730,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F48278F-A549-804C-999D-E15CBB151350}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:CF42"/>
+  <dimension ref="A1:CH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B22"/>
+    <sheetView tabSelected="1" topLeftCell="BL1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="BT19" sqref="BT19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,7 +741,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
@@ -991,8 +990,14 @@
       <c r="CF1" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="CG1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="CH1" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="2" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1243,8 +1248,10 @@
       <c r="CF2" s="1">
         <v>40</v>
       </c>
+      <c r="CG2" s="8"/>
+      <c r="CH2" s="8"/>
     </row>
-    <row r="3" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1333,8 +1340,10 @@
       <c r="CD3" s="1"/>
       <c r="CE3" s="1"/>
       <c r="CF3" s="1"/>
+      <c r="CG3" s="8"/>
+      <c r="CH3" s="8"/>
     </row>
-    <row r="4" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1441,8 +1450,10 @@
       <c r="CD4" s="1"/>
       <c r="CE4" s="1"/>
       <c r="CF4" s="1"/>
+      <c r="CG4" s="8"/>
+      <c r="CH4" s="8"/>
     </row>
-    <row r="5" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1551,8 +1562,10 @@
       <c r="CD5" s="1"/>
       <c r="CE5" s="1"/>
       <c r="CF5" s="1"/>
+      <c r="CG5" s="8"/>
+      <c r="CH5" s="8"/>
     </row>
-    <row r="6" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1661,8 +1674,10 @@
       <c r="CD6" s="1"/>
       <c r="CE6" s="1"/>
       <c r="CF6" s="1"/>
+      <c r="CG6" s="8"/>
+      <c r="CH6" s="8"/>
     </row>
-    <row r="7" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1751,8 +1766,10 @@
       <c r="CD7" s="1"/>
       <c r="CE7" s="1"/>
       <c r="CF7" s="1"/>
+      <c r="CG7" s="8"/>
+      <c r="CH7" s="8"/>
     </row>
-    <row r="8" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1841,8 +1858,10 @@
       <c r="CD8" s="1"/>
       <c r="CE8" s="1"/>
       <c r="CF8" s="1"/>
+      <c r="CG8" s="8"/>
+      <c r="CH8" s="8"/>
     </row>
-    <row r="9" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1931,8 +1950,10 @@
       <c r="CD9" s="1"/>
       <c r="CE9" s="1"/>
       <c r="CF9" s="1"/>
+      <c r="CG9" s="8"/>
+      <c r="CH9" s="8"/>
     </row>
-    <row r="10" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2021,8 +2042,10 @@
       <c r="CD10" s="1"/>
       <c r="CE10" s="1"/>
       <c r="CF10" s="1"/>
+      <c r="CG10" s="8"/>
+      <c r="CH10" s="8"/>
     </row>
-    <row r="11" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2111,8 +2134,10 @@
       <c r="CD11" s="1"/>
       <c r="CE11" s="1"/>
       <c r="CF11" s="1"/>
+      <c r="CG11" s="8"/>
+      <c r="CH11" s="8"/>
     </row>
-    <row r="12" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2203,8 +2228,10 @@
       <c r="CD12" s="1"/>
       <c r="CE12" s="1"/>
       <c r="CF12" s="1"/>
+      <c r="CG12" s="8"/>
+      <c r="CH12" s="8"/>
     </row>
-    <row r="13" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2293,8 +2320,10 @@
       <c r="CD13" s="1"/>
       <c r="CE13" s="1"/>
       <c r="CF13" s="1"/>
+      <c r="CG13" s="8"/>
+      <c r="CH13" s="8"/>
     </row>
-    <row r="14" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2385,8 +2414,10 @@
       <c r="CD14" s="1"/>
       <c r="CE14" s="1"/>
       <c r="CF14" s="1"/>
+      <c r="CG14" s="8"/>
+      <c r="CH14" s="8"/>
     </row>
-    <row r="15" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2475,8 +2506,10 @@
       <c r="CD15" s="1"/>
       <c r="CE15" s="1"/>
       <c r="CF15" s="1"/>
+      <c r="CG15" s="8"/>
+      <c r="CH15" s="8"/>
     </row>
-    <row r="16" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2567,8 +2600,10 @@
       <c r="CD16" s="1"/>
       <c r="CE16" s="1"/>
       <c r="CF16" s="1"/>
+      <c r="CG16" s="8"/>
+      <c r="CH16" s="8"/>
     </row>
-    <row r="17" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2657,8 +2692,10 @@
       <c r="CD17" s="1"/>
       <c r="CE17" s="1"/>
       <c r="CF17" s="1"/>
+      <c r="CG17" s="8"/>
+      <c r="CH17" s="8"/>
     </row>
-    <row r="18" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2749,8 +2786,10 @@
       <c r="CD18" s="1"/>
       <c r="CE18" s="1"/>
       <c r="CF18" s="1"/>
+      <c r="CG18" s="8"/>
+      <c r="CH18" s="8"/>
     </row>
-    <row r="19" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2839,8 +2878,10 @@
       <c r="CD19" s="1"/>
       <c r="CE19" s="1"/>
       <c r="CF19" s="1"/>
+      <c r="CG19" s="8"/>
+      <c r="CH19" s="8"/>
     </row>
-    <row r="20" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -3053,8 +3094,10 @@
       <c r="CD20" s="1"/>
       <c r="CE20" s="1"/>
       <c r="CF20" s="1"/>
+      <c r="CG20" s="8"/>
+      <c r="CH20" s="8"/>
     </row>
-    <row r="21" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -3267,8 +3310,10 @@
       <c r="CD21" s="1"/>
       <c r="CE21" s="1"/>
       <c r="CF21" s="1"/>
+      <c r="CG21" s="8"/>
+      <c r="CH21" s="8"/>
     </row>
-    <row r="22" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -3481,8 +3526,10 @@
       <c r="CD22" s="1"/>
       <c r="CE22" s="1"/>
       <c r="CF22" s="1"/>
+      <c r="CG22" s="8"/>
+      <c r="CH22" s="8"/>
     </row>
-    <row r="23" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -3699,8 +3746,10 @@
       <c r="CD23" s="1"/>
       <c r="CE23" s="1"/>
       <c r="CF23" s="1"/>
+      <c r="CG23" s="8"/>
+      <c r="CH23" s="8"/>
     </row>
-    <row r="24" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -3917,8 +3966,10 @@
       <c r="CD24" s="1"/>
       <c r="CE24" s="1"/>
       <c r="CF24" s="1"/>
+      <c r="CG24" s="8"/>
+      <c r="CH24" s="8"/>
     </row>
-    <row r="25" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -4135,8 +4186,10 @@
       <c r="CD25" s="1"/>
       <c r="CE25" s="1"/>
       <c r="CF25" s="1"/>
+      <c r="CG25" s="8"/>
+      <c r="CH25" s="8"/>
     </row>
-    <row r="26" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -4353,8 +4406,10 @@
       <c r="CD26" s="1"/>
       <c r="CE26" s="1"/>
       <c r="CF26" s="1"/>
+      <c r="CG26" s="8"/>
+      <c r="CH26" s="8"/>
     </row>
-    <row r="27" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -4443,8 +4498,10 @@
       <c r="CD27" s="1"/>
       <c r="CE27" s="1"/>
       <c r="CF27" s="1"/>
+      <c r="CG27" s="8"/>
+      <c r="CH27" s="8"/>
     </row>
-    <row r="28" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -4659,8 +4716,10 @@
       <c r="CD28" s="1"/>
       <c r="CE28" s="1"/>
       <c r="CF28" s="1"/>
+      <c r="CG28" s="8"/>
+      <c r="CH28" s="8"/>
     </row>
-    <row r="29" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -4751,8 +4810,10 @@
       <c r="CD29" s="1"/>
       <c r="CE29" s="1"/>
       <c r="CF29" s="1"/>
+      <c r="CG29" s="8"/>
+      <c r="CH29" s="8"/>
     </row>
-    <row r="30" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -4843,8 +4904,10 @@
       <c r="CD30" s="1"/>
       <c r="CE30" s="1"/>
       <c r="CF30" s="1"/>
+      <c r="CG30" s="8"/>
+      <c r="CH30" s="8"/>
     </row>
-    <row r="31" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -4935,8 +4998,10 @@
       <c r="CD31" s="1"/>
       <c r="CE31" s="1"/>
       <c r="CF31" s="1"/>
+      <c r="CG31" s="8"/>
+      <c r="CH31" s="8"/>
     </row>
-    <row r="32" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -5025,8 +5090,10 @@
       <c r="CD32" s="1"/>
       <c r="CE32" s="1"/>
       <c r="CF32" s="1"/>
+      <c r="CG32" s="8"/>
+      <c r="CH32" s="8"/>
     </row>
-    <row r="33" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -5115,8 +5182,10 @@
       <c r="CD33" s="1"/>
       <c r="CE33" s="1"/>
       <c r="CF33" s="1"/>
+      <c r="CG33" s="8"/>
+      <c r="CH33" s="8"/>
     </row>
-    <row r="34" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -5225,8 +5294,10 @@
       <c r="CD34" s="1"/>
       <c r="CE34" s="1"/>
       <c r="CF34" s="1"/>
+      <c r="CG34" s="8"/>
+      <c r="CH34" s="8"/>
     </row>
-    <row r="35" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -5335,8 +5406,10 @@
       <c r="CD35" s="1"/>
       <c r="CE35" s="1"/>
       <c r="CF35" s="1"/>
+      <c r="CG35" s="8"/>
+      <c r="CH35" s="8"/>
     </row>
-    <row r="36" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -5425,8 +5498,10 @@
       <c r="CD36" s="1"/>
       <c r="CE36" s="1"/>
       <c r="CF36" s="1"/>
+      <c r="CG36" s="8"/>
+      <c r="CH36" s="8"/>
     </row>
-    <row r="37" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -5515,8 +5590,10 @@
       <c r="CD37" s="1"/>
       <c r="CE37" s="1"/>
       <c r="CF37" s="1"/>
+      <c r="CG37" s="8"/>
+      <c r="CH37" s="8"/>
     </row>
-    <row r="38" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -5605,8 +5682,10 @@
       <c r="CD38" s="1"/>
       <c r="CE38" s="1"/>
       <c r="CF38" s="1"/>
+      <c r="CG38" s="8"/>
+      <c r="CH38" s="8"/>
     </row>
-    <row r="39" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -5695,8 +5774,10 @@
       <c r="CD39" s="1"/>
       <c r="CE39" s="1"/>
       <c r="CF39" s="1"/>
+      <c r="CG39" s="8"/>
+      <c r="CH39" s="8"/>
     </row>
-    <row r="40" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -5785,8 +5866,10 @@
       <c r="CD40" s="1"/>
       <c r="CE40" s="1"/>
       <c r="CF40" s="1"/>
+      <c r="CG40" s="8"/>
+      <c r="CH40" s="8"/>
     </row>
-    <row r="41" spans="1:84" ht="20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:86" ht="20" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -5875,96 +5958,284 @@
       <c r="CD41" s="1"/>
       <c r="CE41" s="1"/>
       <c r="CF41" s="1"/>
+      <c r="CG41" s="8"/>
+      <c r="CH41" s="8"/>
     </row>
-    <row r="42" spans="1:84" ht="20" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
+    <row r="42" spans="1:86" ht="20" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
         <v>40</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="8"/>
-      <c r="W42" s="8"/>
-      <c r="X42" s="8"/>
-      <c r="Y42" s="8"/>
-      <c r="Z42" s="8"/>
-      <c r="AA42" s="8"/>
-      <c r="AB42" s="8"/>
-      <c r="AC42" s="8"/>
-      <c r="AD42" s="8"/>
-      <c r="AE42" s="8"/>
-      <c r="AF42" s="8"/>
-      <c r="AG42" s="8"/>
-      <c r="AH42" s="8"/>
-      <c r="AI42" s="8"/>
-      <c r="AJ42" s="8"/>
-      <c r="AK42" s="8"/>
-      <c r="AL42" s="8"/>
-      <c r="AM42" s="8"/>
-      <c r="AN42" s="8"/>
-      <c r="AO42" s="8"/>
-      <c r="AP42" s="8"/>
-      <c r="AQ42" s="8"/>
-      <c r="AR42" s="8"/>
-      <c r="AS42" s="8"/>
-      <c r="AT42" s="8"/>
-      <c r="AU42" s="8"/>
-      <c r="AV42" s="8"/>
-      <c r="AW42" s="8"/>
-      <c r="AX42" s="8"/>
-      <c r="AY42" s="8"/>
-      <c r="AZ42" s="8"/>
-      <c r="BA42" s="8"/>
-      <c r="BB42" s="8"/>
-      <c r="BC42" s="8"/>
-      <c r="BD42" s="8"/>
-      <c r="BE42" s="8"/>
-      <c r="BF42" s="8"/>
-      <c r="BG42" s="8"/>
-      <c r="BH42" s="8"/>
-      <c r="BI42" s="8"/>
-      <c r="BJ42" s="8"/>
-      <c r="BK42" s="8"/>
-      <c r="BL42" s="8"/>
-      <c r="BM42" s="8"/>
-      <c r="BN42" s="8"/>
-      <c r="BO42" s="8"/>
-      <c r="BP42" s="8"/>
-      <c r="BQ42" s="8"/>
-      <c r="BR42" s="8"/>
-      <c r="BS42" s="8"/>
-      <c r="BT42" s="8"/>
-      <c r="BU42" s="8"/>
-      <c r="BV42" s="8"/>
-      <c r="BW42" s="8"/>
-      <c r="BX42" s="8"/>
-      <c r="BY42" s="8"/>
-      <c r="BZ42" s="8"/>
-      <c r="CA42" s="8"/>
-      <c r="CB42" s="8"/>
-      <c r="CC42" s="8"/>
-      <c r="CD42" s="8"/>
-      <c r="CE42" s="8"/>
-      <c r="CF42" s="8"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="1"/>
+      <c r="AF42" s="1"/>
+      <c r="AG42" s="1"/>
+      <c r="AH42" s="1"/>
+      <c r="AI42" s="1"/>
+      <c r="AJ42" s="1"/>
+      <c r="AK42" s="1"/>
+      <c r="AL42" s="1"/>
+      <c r="AM42" s="1"/>
+      <c r="AN42" s="1"/>
+      <c r="AO42" s="1"/>
+      <c r="AP42" s="1"/>
+      <c r="AQ42" s="1"/>
+      <c r="AR42" s="1"/>
+      <c r="AS42" s="1"/>
+      <c r="AT42" s="1"/>
+      <c r="AU42" s="1"/>
+      <c r="AV42" s="1"/>
+      <c r="AW42" s="1"/>
+      <c r="AX42" s="1"/>
+      <c r="AY42" s="1"/>
+      <c r="AZ42" s="1"/>
+      <c r="BA42" s="1"/>
+      <c r="BB42" s="1"/>
+      <c r="BC42" s="1"/>
+      <c r="BD42" s="1"/>
+      <c r="BE42" s="1"/>
+      <c r="BF42" s="1"/>
+      <c r="BG42" s="1"/>
+      <c r="BH42" s="1"/>
+      <c r="BI42" s="1"/>
+      <c r="BJ42" s="1"/>
+      <c r="BK42" s="1"/>
+      <c r="BL42" s="1"/>
+      <c r="BM42" s="1"/>
+      <c r="BN42" s="1"/>
+      <c r="BO42" s="1"/>
+      <c r="BP42" s="1"/>
+      <c r="BQ42" s="1"/>
+      <c r="BR42" s="1"/>
+      <c r="BS42" s="1"/>
+      <c r="BT42" s="1"/>
+      <c r="BU42" s="1"/>
+      <c r="BV42" s="1"/>
+      <c r="BW42" s="1"/>
+      <c r="BX42" s="1"/>
+      <c r="BY42" s="1"/>
+      <c r="BZ42" s="1"/>
+      <c r="CA42" s="1"/>
+      <c r="CB42" s="1"/>
+      <c r="CC42" s="1"/>
+      <c r="CD42" s="1"/>
+      <c r="CE42" s="1"/>
+      <c r="CF42" s="1"/>
+      <c r="CG42" s="8"/>
+      <c r="CH42" s="8"/>
+    </row>
+    <row r="43" spans="1:86" ht="20" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>41</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="8"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
+      <c r="Y43" s="8"/>
+      <c r="Z43" s="8"/>
+      <c r="AA43" s="8"/>
+      <c r="AB43" s="8"/>
+      <c r="AC43" s="8"/>
+      <c r="AD43" s="8"/>
+      <c r="AE43" s="8"/>
+      <c r="AF43" s="8"/>
+      <c r="AG43" s="8"/>
+      <c r="AH43" s="8"/>
+      <c r="AI43" s="8"/>
+      <c r="AJ43" s="8"/>
+      <c r="AK43" s="8"/>
+      <c r="AL43" s="8"/>
+      <c r="AM43" s="8"/>
+      <c r="AN43" s="8"/>
+      <c r="AO43" s="8"/>
+      <c r="AP43" s="8"/>
+      <c r="AQ43" s="8"/>
+      <c r="AR43" s="8"/>
+      <c r="AS43" s="8"/>
+      <c r="AT43" s="8"/>
+      <c r="AU43" s="8"/>
+      <c r="AV43" s="8"/>
+      <c r="AW43" s="8"/>
+      <c r="AX43" s="8"/>
+      <c r="AY43" s="8"/>
+      <c r="AZ43" s="8"/>
+      <c r="BA43" s="8"/>
+      <c r="BB43" s="8"/>
+      <c r="BC43" s="8"/>
+      <c r="BD43" s="8"/>
+      <c r="BE43" s="8"/>
+      <c r="BF43" s="8"/>
+      <c r="BG43" s="8"/>
+      <c r="BH43" s="8"/>
+      <c r="BI43" s="8"/>
+      <c r="BJ43" s="8"/>
+      <c r="BK43" s="8"/>
+      <c r="BL43" s="8"/>
+      <c r="BM43" s="8"/>
+      <c r="BN43" s="8"/>
+      <c r="BO43" s="8"/>
+      <c r="BP43" s="8"/>
+      <c r="BQ43" s="8"/>
+      <c r="BR43" s="8"/>
+      <c r="BS43" s="8"/>
+      <c r="BT43" s="8"/>
+      <c r="BU43" s="8"/>
+      <c r="BV43" s="8"/>
+      <c r="BW43" s="8"/>
+      <c r="BX43" s="8"/>
+      <c r="BY43" s="8"/>
+      <c r="BZ43" s="8"/>
+      <c r="CA43" s="8"/>
+      <c r="CB43" s="8"/>
+      <c r="CC43" s="8"/>
+      <c r="CD43" s="8"/>
+      <c r="CE43" s="8"/>
+      <c r="CF43" s="8"/>
+      <c r="CG43" s="8"/>
+      <c r="CH43" s="8"/>
+    </row>
+    <row r="44" spans="1:86" ht="20" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>42</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="8"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="8"/>
+      <c r="Y44" s="8"/>
+      <c r="Z44" s="8"/>
+      <c r="AA44" s="8"/>
+      <c r="AB44" s="8"/>
+      <c r="AC44" s="8"/>
+      <c r="AD44" s="8"/>
+      <c r="AE44" s="8"/>
+      <c r="AF44" s="8"/>
+      <c r="AG44" s="8"/>
+      <c r="AH44" s="8"/>
+      <c r="AI44" s="8"/>
+      <c r="AJ44" s="8"/>
+      <c r="AK44" s="8"/>
+      <c r="AL44" s="8"/>
+      <c r="AM44" s="8"/>
+      <c r="AN44" s="8"/>
+      <c r="AO44" s="8"/>
+      <c r="AP44" s="8"/>
+      <c r="AQ44" s="8"/>
+      <c r="AR44" s="8"/>
+      <c r="AS44" s="8"/>
+      <c r="AT44" s="8"/>
+      <c r="AU44" s="8"/>
+      <c r="AV44" s="8"/>
+      <c r="AW44" s="8"/>
+      <c r="AX44" s="8"/>
+      <c r="AY44" s="8"/>
+      <c r="AZ44" s="8"/>
+      <c r="BA44" s="8"/>
+      <c r="BB44" s="8"/>
+      <c r="BC44" s="8"/>
+      <c r="BD44" s="8"/>
+      <c r="BE44" s="8"/>
+      <c r="BF44" s="8"/>
+      <c r="BG44" s="8"/>
+      <c r="BH44" s="8"/>
+      <c r="BI44" s="8"/>
+      <c r="BJ44" s="8"/>
+      <c r="BK44" s="8"/>
+      <c r="BL44" s="8"/>
+      <c r="BM44" s="8"/>
+      <c r="BN44" s="8"/>
+      <c r="BO44" s="8"/>
+      <c r="BP44" s="8"/>
+      <c r="BQ44" s="8"/>
+      <c r="BR44" s="8"/>
+      <c r="BS44" s="8"/>
+      <c r="BT44" s="8"/>
+      <c r="BU44" s="8"/>
+      <c r="BV44" s="8"/>
+      <c r="BW44" s="8"/>
+      <c r="BX44" s="8"/>
+      <c r="BY44" s="8"/>
+      <c r="BZ44" s="8"/>
+      <c r="CA44" s="8"/>
+      <c r="CB44" s="8"/>
+      <c r="CC44" s="8"/>
+      <c r="CD44" s="8"/>
+      <c r="CE44" s="8"/>
+      <c r="CF44" s="8"/>
+      <c r="CG44" s="8"/>
+      <c r="CH44" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>